<commit_message>
Update study.xlsx + dataSets type.en renamed
</commit_message>
<xml_diff>
--- a/data/dataSets/dataSets.xlsx
+++ b/data/dataSets/dataSets.xlsx
@@ -66,9 +66,6 @@
     <t>1, 2</t>
   </si>
   <si>
-    <t>Personal Record</t>
-  </si>
-  <si>
     <t>format.de</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Individual data DZHW Graduate Panel 2009 - first wave</t>
+  </si>
+  <si>
+    <t>Individual Data</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +547,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -561,22 +561,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>15</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="10">
         <v>1049</v>
@@ -645,10 +645,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="10">
         <v>10494</v>
@@ -665,10 +665,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="10">
         <v>10494</v>
@@ -685,10 +685,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="6">
         <v>1</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="10">
         <v>10494</v>
@@ -705,10 +705,10 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
@@ -775,10 +775,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -787,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
+ annotations.de/.en for all projects
</commit_message>
<xml_diff>
--- a/data/dataSets/dataSets.xlsx
+++ b/data/dataSets/dataSets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>number</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Individual Data</t>
+  </si>
+  <si>
+    <t>annotations.de</t>
+  </si>
+  <si>
+    <t>annotations.en</t>
   </si>
 </sst>
 </file>
@@ -512,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +536,7 @@
     <col min="9" max="1027" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,8 +561,14 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -582,11 +594,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="D4" s="2"/>
     </row>

</xml_diff>

<commit_message>
Release abs09 2nd wave
</commit_message>
<xml_diff>
--- a/data/dataSets/dataSets.xlsx
+++ b/data/dataSets/dataSets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dataSets" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>number</t>
   </si>
@@ -63,97 +63,142 @@
     <t>download-suf</t>
   </si>
   <si>
+    <t>format.de</t>
+  </si>
+  <si>
+    <t>format.en</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>breit</t>
+  </si>
+  <si>
+    <t>wide</t>
+  </si>
+  <si>
+    <t>Kann ohne Datennutzungsvertrag heruntergeladen werden</t>
+  </si>
+  <si>
+    <t>Kann nach Abschluss eines Datennutzungsvertrags heruntergeladen werden</t>
+  </si>
+  <si>
+    <t>Kann über Remote Desktop genutzt werden</t>
+  </si>
+  <si>
+    <t>Ist am Gastwissenschaftlerarbeitsplatz im DZHW in Hannover verfügbar</t>
+  </si>
+  <si>
+    <t>can be downloaded without a data use agreement</t>
+  </si>
+  <si>
+    <t>can be downloaded after the conclusion of a data use agreement</t>
+  </si>
+  <si>
+    <t>can be used via remote desktop</t>
+  </si>
+  <si>
+    <t>available at the workspace for visiting scientists at the DZHW in Hannover</t>
+  </si>
+  <si>
+    <t>Individual Data</t>
+  </si>
+  <si>
+    <t>annotations.de</t>
+  </si>
+  <si>
+    <t>annotations.en</t>
+  </si>
+  <si>
+    <t>Personendatensatz DZHW-Absolventenpanel 2009</t>
+  </si>
+  <si>
+    <t>Individual data DZHW Graduate Panel 2009</t>
+  </si>
+  <si>
+    <t>Episodendatensatz</t>
+  </si>
+  <si>
+    <t>Spell Data</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>Episodendatensatz DZHW-Absolventenpanel 2009</t>
+  </si>
+  <si>
+    <t>Spell data DZHW Graduate Panel 2009</t>
+  </si>
+  <si>
+    <t>gra2009_p_c_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_p_d_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_p_r_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_p_o_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_e_c_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_e_d_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_e_r_1-0-0</t>
+  </si>
+  <si>
+    <t>gra2009_e_o_1-0-0</t>
+  </si>
+  <si>
+    <t>citationHint.de</t>
+  </si>
+  <si>
+    <t>citationHint.en</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_c_1-0-0 , released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_d_1-0-0 , released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_r_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_e_c_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_e_d_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_e_r_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_e_o_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
+    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_o_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+  </si>
+  <si>
     <t>1, 2</t>
   </si>
   <si>
-    <t>format.de</t>
-  </si>
-  <si>
-    <t>format.en</t>
-  </si>
-  <si>
-    <t>filename</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>breit</t>
-  </si>
-  <si>
-    <t>wide</t>
-  </si>
-  <si>
-    <t>Kann ohne Datennutzungsvertrag heruntergeladen werden</t>
-  </si>
-  <si>
-    <t>Kann nach Abschluss eines Datennutzungsvertrags heruntergeladen werden</t>
-  </si>
-  <si>
-    <t>Kann über Remote Desktop genutzt werden</t>
-  </si>
-  <si>
-    <t>Ist am Gastwissenschaftlerarbeitsplatz im DZHW in Hannover verfügbar</t>
-  </si>
-  <si>
-    <t>gra2009_p_w1_c_1-0-0</t>
-  </si>
-  <si>
-    <t>gra2009_p_w1_d_1-0-0</t>
-  </si>
-  <si>
-    <t>gra2009_p_w1_r_1-0-0</t>
-  </si>
-  <si>
-    <t>gra2009_p_w1_o_1-0-0</t>
-  </si>
-  <si>
-    <t>can be downloaded without a data use agreement</t>
-  </si>
-  <si>
-    <t>can be downloaded after the conclusion of a data use agreement</t>
-  </si>
-  <si>
-    <t>can be used via remote desktop</t>
-  </si>
-  <si>
-    <t>available at the workspace for visiting scientists at the DZHW in Hannover</t>
-  </si>
-  <si>
-    <t>Personendatensatz DZHW-Absolventenpanel 2009 - erste Welle</t>
-  </si>
-  <si>
-    <t>Individual data DZHW Graduate Panel 2009 - first wave</t>
-  </si>
-  <si>
-    <t>Individual Data</t>
-  </si>
-  <si>
-    <t>annotations.de</t>
-  </si>
-  <si>
-    <t>annotations.en</t>
-  </si>
-  <si>
-    <t>citationHint.de</t>
-  </si>
-  <si>
-    <t>citationHint.en</t>
-  </si>
-  <si>
-    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_w1_c_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
-  </si>
-  <si>
-    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_w1_d_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
-  </si>
-  <si>
-    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_w1_r_1-0-0 , released 2017. Hannover: FDZ-DZHW.</t>
-  </si>
-  <si>
-    <t>Brandt, G., Briedis, K., Fabian, G., Klüver, S., Rehn, T. &amp; Trommer, M. (2016). DZHW-Absolventenpanel 2009. Aufbereitet durch Baillet, F., Franken, A. &amp; Weber, A., doi: 10.21249/DZHW:gra2009:1.0.0, gra2009_p_w1_o_1-0-0, released 2017. Hannover: FDZ-DZHW.</t>
+    <t>1, 2, 3, 4</t>
   </si>
 </sst>
 </file>
@@ -216,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -234,9 +279,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Erklärender Text 2" xfId="1"/>
@@ -541,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +595,7 @@
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="1" customWidth="1"/>
     <col min="9" max="1027" width="10.5703125"/>
   </cols>
   <sheetData>
@@ -574,19 +616,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -594,30 +636,52 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="D3" s="3"/>
+      <c r="G3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
@@ -633,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +708,8 @@
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="82.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="1022" width="10.5703125"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="1022" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -667,15 +732,15 @@
         <v>9</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B2" s="10">
         <v>1049</v>
@@ -684,21 +749,21 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>42</v>
+      <c r="G2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B3" s="10">
         <v>10494</v>
@@ -707,21 +772,21 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>43</v>
+      <c r="G3" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B4" s="10">
         <v>10494</v>
@@ -730,21 +795,21 @@
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>44</v>
+      <c r="G4" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B5" s="10">
         <v>10494</v>
@@ -753,22 +818,110 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B6" s="10">
+        <v>3735</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="10">
+        <v>36841</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="10">
+        <v>36841</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="10">
+        <v>36841</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
@@ -826,10 +979,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -838,7 +991,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
subdataset: chnage description for download - cuf
</commit_message>
<xml_diff>
--- a/data/dataSets/dataSets.xlsx
+++ b/data/dataSets/dataSets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="12555" yWindow="45" windowWidth="22770" windowHeight="12705" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dataSets" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>wide</t>
   </si>
   <si>
-    <t>Kann ohne Datennutzungsvertrag heruntergeladen werden</t>
-  </si>
-  <si>
     <t>Kann nach Abschluss eines Datennutzungsvertrags heruntergeladen werden</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Ist am Gastwissenschaftlerarbeitsplatz im DZHW in Hannover verfügbar</t>
   </si>
   <si>
-    <t>can be downloaded without a data use agreement</t>
-  </si>
-  <si>
     <t>can be downloaded after the conclusion of a data use agreement</t>
   </si>
   <si>
@@ -199,13 +193,19 @@
   </si>
   <si>
     <t>1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>Kann nach einer Registrierung ohne Datennutzungsvertrag heruntergeladen werden</t>
+  </si>
+  <si>
+    <t>can be downloaded after registration without a data use agreement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -232,6 +232,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -261,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -279,6 +286,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Erklärender Text 2" xfId="1"/>
@@ -583,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -625,10 +635,10 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -636,16 +646,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>20</v>
@@ -654,7 +664,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -662,25 +672,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -697,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,15 +742,15 @@
         <v>9</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="10">
         <v>1049</v>
@@ -749,21 +759,21 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>26</v>
+        <v>59</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="10">
         <v>10494</v>
@@ -772,21 +782,21 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="10">
         <v>10494</v>
@@ -795,21 +805,21 @@
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="6">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="10">
         <v>10494</v>
@@ -818,21 +828,21 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="10">
         <v>3735</v>
@@ -841,21 +851,21 @@
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>26</v>
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F6" s="6">
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="10">
         <v>36841</v>
@@ -864,21 +874,21 @@
         <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F7" s="6">
         <v>2</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="10">
         <v>36841</v>
@@ -887,21 +897,21 @@
         <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="6">
         <v>2</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="10">
         <v>36841</v>
@@ -910,16 +920,16 @@
         <v>12</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6">
         <v>2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>